<commit_message>
Error message for n students n codewords
</commit_message>
<xml_diff>
--- a/Documentation/Data/studentdetails.xlsx
+++ b/Documentation/Data/studentdetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sravya\Fall\GDP\MVP3\CodeWord\Documentation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sravya\Fall\GDP\push1118\CodeWord\Documentation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{08A27BF5-FFF7-46EB-8436-D6973C823F18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{69BEDA58-87A9-42C9-A37C-3E811D4A552D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{95C39AE2-582D-4A00-97E8-546D466C3CF2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="44">
   <si>
     <t>Email</t>
   </si>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F26843E-3266-4216-A860-798E2A23D903}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,6 +817,678 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -841,8 +1513,92 @@
     <hyperlink ref="A20" r:id="rId19" display="mailto:s531384@nwmissouri.edu" xr:uid="{A5F59E60-823F-43E1-9E0C-27B2FD3BDACC}"/>
     <hyperlink ref="A21" r:id="rId20" display="mailto:hoot@nwmissouri.edu" xr:uid="{E8E9D016-305A-40C0-A243-62E6B41268A0}"/>
     <hyperlink ref="A22" r:id="rId21" display="mailto:dcase@nwmissouri.edu" xr:uid="{B5CD4374-65D1-4FFB-8B39-24E8A6CC15AE}"/>
+    <hyperlink ref="A23" r:id="rId22" display="mailto:s531519@nwmissouri.edu" xr:uid="{B00D4BC2-CBC1-41CB-AA3A-6332FCEB5758}"/>
+    <hyperlink ref="A24" r:id="rId23" display="mailto:s530742@nwmissouri.edu" xr:uid="{49B9C94B-486B-4C20-B817-7BF6650093A8}"/>
+    <hyperlink ref="A25" r:id="rId24" display="mailto:s531495@nwmissouri.edu" xr:uid="{68A5EC6B-D7DB-43D3-8F4A-91D0291A620E}"/>
+    <hyperlink ref="A26" r:id="rId25" display="mailto:s531367@nwmissouri.edu" xr:uid="{07D9C5A6-B37D-49FD-ABF8-CA458C3E6D81}"/>
+    <hyperlink ref="A27" r:id="rId26" display="mailto:s531496@nwmissouri.edu" xr:uid="{B794FF9B-6925-440F-B31B-84FCDBD18753}"/>
+    <hyperlink ref="A28" r:id="rId27" display="mailto:s531369@nwmissouri.edu" xr:uid="{4ED13DD3-490D-4A7E-819F-09882F932C91}"/>
+    <hyperlink ref="A29" r:id="rId28" display="mailto:s531499@nwmissouri.edu" xr:uid="{FE600552-C3F7-4501-BCFD-4834F14346CE}"/>
+    <hyperlink ref="A30" r:id="rId29" display="mailto:s531500@nwmissouri.edu" xr:uid="{947D6C97-D1E0-4D85-B903-E1A3951AFB29}"/>
+    <hyperlink ref="A31" r:id="rId30" display="mailto:s531372@nwmissouri.edu" xr:uid="{81E0EF83-F7A4-40A3-B808-63DA81D5E87E}"/>
+    <hyperlink ref="A32" r:id="rId31" display="mailto:s530473@nwmissouri.edu" xr:uid="{758A4E06-A45E-4191-8702-8196765C5499}"/>
+    <hyperlink ref="A33" r:id="rId32" display="mailto:s531439@nwmissouri.edu" xr:uid="{27020D04-4929-400D-94B0-4F951D68821B}"/>
+    <hyperlink ref="A34" r:id="rId33" display="mailto:s531503@nwmissouri.edu" xr:uid="{2C63D071-1E09-4D86-8167-8F0B36F8944D}"/>
+    <hyperlink ref="A35" r:id="rId34" display="mailto:s531373@nwmissouri.edu" xr:uid="{844C7821-3BBC-4C88-90D7-10F7EF92BE89}"/>
+    <hyperlink ref="A36" r:id="rId35" display="mailto:s531507@nwmissouri.edu" xr:uid="{D4ADB331-83D8-4F62-A790-674354B745D4}"/>
+    <hyperlink ref="A37" r:id="rId36" display="mailto:s531508@nwmissouri.edu" xr:uid="{ECA9C8F1-EC80-48B9-A0C1-B7DEFCF932E0}"/>
+    <hyperlink ref="A38" r:id="rId37" display="mailto:s531382@nwmissouri.edu" xr:uid="{B8ACF360-1293-4A69-A60E-6635CC668D1D}"/>
+    <hyperlink ref="A39" r:id="rId38" display="mailto:mwoolery@nwmissouri.edu" xr:uid="{30347591-B942-46AB-8821-3803F751CF89}"/>
+    <hyperlink ref="A40" r:id="rId39" display="mailto:s531383@nwmissouri.edu" xr:uid="{B923096E-A9AC-48C2-A119-580DF0634845}"/>
+    <hyperlink ref="A41" r:id="rId40" display="mailto:s531384@nwmissouri.edu" xr:uid="{50AFE385-2962-4FEA-860D-17167F9BE586}"/>
+    <hyperlink ref="A42" r:id="rId41" display="mailto:hoot@nwmissouri.edu" xr:uid="{A7FC26C3-61C8-456A-9CE2-0089889310E9}"/>
+    <hyperlink ref="A43" r:id="rId42" display="mailto:dcase@nwmissouri.edu" xr:uid="{88FAF70F-BD34-4C5E-9284-39C6931F175F}"/>
+    <hyperlink ref="A44" r:id="rId43" display="mailto:s531519@nwmissouri.edu" xr:uid="{0BAAAB30-EA39-4970-93EE-3B68D15585B5}"/>
+    <hyperlink ref="A45" r:id="rId44" display="mailto:s530742@nwmissouri.edu" xr:uid="{A6526348-0513-4CFC-9A3A-634741535152}"/>
+    <hyperlink ref="A46" r:id="rId45" display="mailto:s531495@nwmissouri.edu" xr:uid="{B988619A-15DB-4CB7-9930-8F6D2CABC704}"/>
+    <hyperlink ref="A47" r:id="rId46" display="mailto:s531367@nwmissouri.edu" xr:uid="{C402A4B6-9D87-4177-B1F3-D3D665058047}"/>
+    <hyperlink ref="A48" r:id="rId47" display="mailto:s531496@nwmissouri.edu" xr:uid="{E4F53E8A-DD87-468C-8EE8-1F216F67364D}"/>
+    <hyperlink ref="A49" r:id="rId48" display="mailto:s531369@nwmissouri.edu" xr:uid="{1297CE88-B24B-4D0E-A247-30B9EC69AB91}"/>
+    <hyperlink ref="A50" r:id="rId49" display="mailto:s531499@nwmissouri.edu" xr:uid="{C496B460-CD5A-4601-86A2-05E6CB1DEC09}"/>
+    <hyperlink ref="A51" r:id="rId50" display="mailto:s531500@nwmissouri.edu" xr:uid="{82DF3437-287A-4970-B620-C13E3FA53823}"/>
+    <hyperlink ref="A52" r:id="rId51" display="mailto:s531372@nwmissouri.edu" xr:uid="{16196F36-3D8A-4813-864B-C829BD378427}"/>
+    <hyperlink ref="A53" r:id="rId52" display="mailto:s530473@nwmissouri.edu" xr:uid="{A1EAF1FB-FC16-4718-BBCB-F70BC303CE5B}"/>
+    <hyperlink ref="A54" r:id="rId53" display="mailto:s531439@nwmissouri.edu" xr:uid="{46C35334-5284-4E69-B5E3-F38778CE65C3}"/>
+    <hyperlink ref="A55" r:id="rId54" display="mailto:s531503@nwmissouri.edu" xr:uid="{B7A00A54-AE61-4FAD-BB7B-01CC81FD48CC}"/>
+    <hyperlink ref="A56" r:id="rId55" display="mailto:s531373@nwmissouri.edu" xr:uid="{0825061F-8174-4F73-9CE1-A0D339D36D01}"/>
+    <hyperlink ref="A57" r:id="rId56" display="mailto:s531507@nwmissouri.edu" xr:uid="{0B176DDC-FEBC-4ACD-A449-ACECF907409F}"/>
+    <hyperlink ref="A58" r:id="rId57" display="mailto:s531508@nwmissouri.edu" xr:uid="{3F69ACE0-8BDE-496D-ABFA-613BB20DFCBB}"/>
+    <hyperlink ref="A59" r:id="rId58" display="mailto:s531382@nwmissouri.edu" xr:uid="{C219E083-D3E8-4979-BE4F-13522DB56C2E}"/>
+    <hyperlink ref="A60" r:id="rId59" display="mailto:mwoolery@nwmissouri.edu" xr:uid="{2E7F5221-5B9A-41CB-9224-7ED8097579B9}"/>
+    <hyperlink ref="A61" r:id="rId60" display="mailto:s531383@nwmissouri.edu" xr:uid="{BDE2A1AB-40EB-4D58-80C6-6AD3D0A96017}"/>
+    <hyperlink ref="A62" r:id="rId61" display="mailto:s531384@nwmissouri.edu" xr:uid="{C976A8F0-360A-4AF8-AC18-23A253D723B5}"/>
+    <hyperlink ref="A63" r:id="rId62" display="mailto:hoot@nwmissouri.edu" xr:uid="{BC22107F-F596-4DD9-ACBB-1366C251C22E}"/>
+    <hyperlink ref="A64" r:id="rId63" display="mailto:dcase@nwmissouri.edu" xr:uid="{4BFC0C46-E98A-4E0B-87E0-0980CBB06DC2}"/>
+    <hyperlink ref="A65" r:id="rId64" display="mailto:s531519@nwmissouri.edu" xr:uid="{E670B3D0-0AEB-4AE6-AA34-C2BF6AF022C4}"/>
+    <hyperlink ref="A66" r:id="rId65" display="mailto:s530742@nwmissouri.edu" xr:uid="{0BB56B78-DE5D-4F3B-AC34-B5633289E47F}"/>
+    <hyperlink ref="A67" r:id="rId66" display="mailto:s531495@nwmissouri.edu" xr:uid="{8B9911B0-0BA5-416A-B398-AD3DE4FF58DA}"/>
+    <hyperlink ref="A68" r:id="rId67" display="mailto:s531367@nwmissouri.edu" xr:uid="{57ADC763-3C72-4E49-BCC7-6C58B9ED2CD1}"/>
+    <hyperlink ref="A69" r:id="rId68" display="mailto:s531496@nwmissouri.edu" xr:uid="{55599037-E6D1-41B6-B95D-320F10D4B12F}"/>
+    <hyperlink ref="A70" r:id="rId69" display="mailto:s531369@nwmissouri.edu" xr:uid="{C1E7063E-9167-492E-9D8A-C9536CCCA19D}"/>
+    <hyperlink ref="A71" r:id="rId70" display="mailto:s531499@nwmissouri.edu" xr:uid="{181BC610-F9C5-4771-8063-2DCD9B68EBD0}"/>
+    <hyperlink ref="A72" r:id="rId71" display="mailto:s531500@nwmissouri.edu" xr:uid="{21441BAF-6220-4C4D-9067-11F460A9466D}"/>
+    <hyperlink ref="A73" r:id="rId72" display="mailto:s531372@nwmissouri.edu" xr:uid="{5DCB86C0-D143-4F3B-B7A6-A7E056CB52C9}"/>
+    <hyperlink ref="A74" r:id="rId73" display="mailto:s530473@nwmissouri.edu" xr:uid="{2A8ACEFB-108D-4B75-BE94-E1A216811B12}"/>
+    <hyperlink ref="A75" r:id="rId74" display="mailto:s531439@nwmissouri.edu" xr:uid="{8CF16B8B-2FDA-48D3-B394-74B9DDC43F73}"/>
+    <hyperlink ref="A76" r:id="rId75" display="mailto:s531503@nwmissouri.edu" xr:uid="{929FBE00-BC8D-4157-BD90-B1CAF4F14EFB}"/>
+    <hyperlink ref="A77" r:id="rId76" display="mailto:s531373@nwmissouri.edu" xr:uid="{26ABFF7B-023D-4840-9D41-2D682F28E5E3}"/>
+    <hyperlink ref="A78" r:id="rId77" display="mailto:s531507@nwmissouri.edu" xr:uid="{3496054E-B215-4CEF-88A4-DA66620E6872}"/>
+    <hyperlink ref="A79" r:id="rId78" display="mailto:s531508@nwmissouri.edu" xr:uid="{FC6C5867-3161-4180-B41B-88DFAB994279}"/>
+    <hyperlink ref="A80" r:id="rId79" display="mailto:s531382@nwmissouri.edu" xr:uid="{35FADB40-E0D7-4F60-B7E9-4A1BB1442C43}"/>
+    <hyperlink ref="A81" r:id="rId80" display="mailto:mwoolery@nwmissouri.edu" xr:uid="{4DD6D3F8-3B30-470E-9BCD-F50A7AB47CEB}"/>
+    <hyperlink ref="A82" r:id="rId81" display="mailto:s531383@nwmissouri.edu" xr:uid="{D449BF34-36CA-4FD1-B41F-60B3A47EE169}"/>
+    <hyperlink ref="A83" r:id="rId82" display="mailto:s531384@nwmissouri.edu" xr:uid="{69BD3387-8FA1-4D0D-8562-6A9889D8E7E9}"/>
+    <hyperlink ref="A84" r:id="rId83" display="mailto:hoot@nwmissouri.edu" xr:uid="{1F2238F2-ADBD-4D4D-A7D9-80E25152D3AE}"/>
+    <hyperlink ref="A85" r:id="rId84" display="mailto:dcase@nwmissouri.edu" xr:uid="{205DC9E8-221D-4D10-B8FD-AC9E5A257C12}"/>
+    <hyperlink ref="A86" r:id="rId85" display="mailto:s531519@nwmissouri.edu" xr:uid="{79567A31-75F3-462C-BE3B-FBF52BB7D52E}"/>
+    <hyperlink ref="A87" r:id="rId86" display="mailto:s530742@nwmissouri.edu" xr:uid="{3EDE4975-C10E-4974-BB63-4CE9B6344A70}"/>
+    <hyperlink ref="A88" r:id="rId87" display="mailto:s531495@nwmissouri.edu" xr:uid="{CD72FFB1-7FEC-46DD-919F-7BCBB8D503E3}"/>
+    <hyperlink ref="A89" r:id="rId88" display="mailto:s531367@nwmissouri.edu" xr:uid="{EAE1BB0C-3FD9-473B-90A9-93299A1F0F25}"/>
+    <hyperlink ref="A90" r:id="rId89" display="mailto:s531496@nwmissouri.edu" xr:uid="{BDCCDF1D-C25D-4282-B4E1-2EAEF64E9755}"/>
+    <hyperlink ref="A91" r:id="rId90" display="mailto:s531369@nwmissouri.edu" xr:uid="{BAB7F7E1-3536-4C22-B1E5-A0556C180745}"/>
+    <hyperlink ref="A92" r:id="rId91" display="mailto:s531499@nwmissouri.edu" xr:uid="{9CEC3E6A-E326-46B4-AD63-942491C81CF7}"/>
+    <hyperlink ref="A93" r:id="rId92" display="mailto:s531500@nwmissouri.edu" xr:uid="{019B0DA3-C503-480F-8D47-B87BA016B814}"/>
+    <hyperlink ref="A94" r:id="rId93" display="mailto:s531372@nwmissouri.edu" xr:uid="{1E7D7FD1-C685-48CE-88FC-59210985A21B}"/>
+    <hyperlink ref="A95" r:id="rId94" display="mailto:s530473@nwmissouri.edu" xr:uid="{5C624499-78D3-45E6-9C07-876518DD91BB}"/>
+    <hyperlink ref="A96" r:id="rId95" display="mailto:s531439@nwmissouri.edu" xr:uid="{BDB00D30-21EE-4E2C-A8B7-2A279958B63E}"/>
+    <hyperlink ref="A97" r:id="rId96" display="mailto:s531503@nwmissouri.edu" xr:uid="{1BD4E636-7F9E-4DEA-98F5-F641B40F56E3}"/>
+    <hyperlink ref="A98" r:id="rId97" display="mailto:s531373@nwmissouri.edu" xr:uid="{D7F885CD-781C-44C8-A44C-FCC90A218B9A}"/>
+    <hyperlink ref="A99" r:id="rId98" display="mailto:s531507@nwmissouri.edu" xr:uid="{A1C7256D-F7C0-41A3-87C4-8B2026F2A2EC}"/>
+    <hyperlink ref="A100" r:id="rId99" display="mailto:s531508@nwmissouri.edu" xr:uid="{12947EE6-E0B1-4C8D-85E7-EDC9C8A05D52}"/>
+    <hyperlink ref="A101" r:id="rId100" display="mailto:s531382@nwmissouri.edu" xr:uid="{83892708-6680-40CA-BF96-C51BA8E04754}"/>
+    <hyperlink ref="A102" r:id="rId101" display="mailto:mwoolery@nwmissouri.edu" xr:uid="{8B188589-78EC-4821-ADB1-51164F7135D1}"/>
+    <hyperlink ref="A103" r:id="rId102" display="mailto:s531383@nwmissouri.edu" xr:uid="{6108AF4F-7413-4F6D-A059-2BC4CD2353E5}"/>
+    <hyperlink ref="A104" r:id="rId103" display="mailto:s531384@nwmissouri.edu" xr:uid="{80841051-45FC-402A-8949-0CC9131B2449}"/>
+    <hyperlink ref="A105" r:id="rId104" display="mailto:hoot@nwmissouri.edu" xr:uid="{9AC7D0E6-EA9B-4451-B95A-051D476FC342}"/>
+    <hyperlink ref="A106" r:id="rId105" display="mailto:dcase@nwmissouri.edu" xr:uid="{A9EFBCBF-4E98-4D12-B57A-0DF56DFE30C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId106"/>
 </worksheet>
 </file>
</xml_diff>